<commit_message>
edit student , excel import formatted feature added
</commit_message>
<xml_diff>
--- a/static/admission/student_import_template.xlsx
+++ b/static/admission/student_import_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/AB3AC2199F7FDAF4/Documents/MRJ/sms_project/static/admission/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrjji\OneDrive\Documents\MRJ\sms_project\static\admission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{DAD6D078-BF79-4AC6-AF6A-9942BF1C7304}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{F09F04F8-3D60-4384-BC6F-6A90FFE3AC6E}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{DAD6D078-BF79-4AC6-AF6A-9942BF1C7304}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{FE2F2D85-90D5-43E6-A290-AE60DF96E531}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5904" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>full_name</t>
   </si>
@@ -65,42 +65,6 @@
   </si>
   <si>
     <t>section</t>
-  </si>
-  <si>
-    <t>Mrityunjay Pandey</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>general</t>
-  </si>
-  <si>
-    <t>Hindu</t>
-  </si>
-  <si>
-    <t>9876543210</t>
-  </si>
-  <si>
-    <t>123456789012</t>
-  </si>
-  <si>
-    <t>Ramesh Pandey</t>
-  </si>
-  <si>
-    <t>Sita Pandey</t>
-  </si>
-  <si>
-    <t>Teacher</t>
-  </si>
-  <si>
-    <t>2024-25</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Class 7</t>
   </si>
 </sst>
 </file>
@@ -139,9 +103,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,123 +416,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="1">
-        <v>39521</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="1">
-        <v>45820</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" t="s">
-        <v>25</v>
-      </c>
+      <c r="B2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="q2Tm/6LcZ9GP4ONIsBdSMWSfCZDuilSo4EZHP4QWXPPE+/IrraYAY/cFuPdnhEqT5aWLtt+L5pQjvLrJ0OiDcQ==" saltValue="4SWujj64fW3Yw0pBt0Aa4w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>